<commit_message>
Send report to user via email
</commit_message>
<xml_diff>
--- a/sentiment-analysis.xlsx
+++ b/sentiment-analysis.xlsx
@@ -25,25 +25,25 @@
     <x:t>Sentiment</x:t>
   </x:si>
   <x:si>
-    <x:t>No Time to Die</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bond has left active service and is enjoying a tranquil life in Jamaica. His peace is short-lived when his old friend Felix Leiter from the CIA turns up asking for help. The mission to rescue a kidnapped scientist turns out to be far more treacherous than expected, leading Bond onto the trail of a mysterious villain armed with dangerous new technology.</x:t>
+    <x:t>Free Guy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A bank teller called Guy realizes he is a background character in an open world video game called Free City that will soon go offline.</x:t>
   </x:si>
   <x:si>
     <x:t>neutral</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Chernobyl: Abyss </x:t>
-  </x:si>
-  <x:si>
-    <x:t>The aftermath of a shocking explosion at the Chernobyl nuclear power station made hundreds of people sacrifice their lives to clean up the site of the catastrophe and to successfully prevent an even bigger disaster that could have turned a large part of the European continent into an uninhabitable exclusion zone. This is their story.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">The Simpsons in Plusaversary </x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Simpsons host a Disney+ Day party and everyone is on the list… except Homer. With friends from across the service and music fit for a Disney Princess, Plusaversary is Springfield's event of the year.</x:t>
+    <x:t xml:space="preserve">Eternals </x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Eternals are a team of ancient aliens who have been living on Earth in secret for thousands of years. When an unexpected tragedy forces them out of the shadows, they are forced to reunite against mankind’s most ancient enemy, the Deviants.</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Spider-Man: No Way Home </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Peter Parker is unmasked and no longer able to separate his normal life from the high-stakes of being a Super Hero. When he asks for help from Doctor Strange the stakes become even more dangerous, forcing him to discover what it truly means to be Spider-Man.</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>